<commit_message>
Actualizar mensajes: añadir nuevos y eliminar duplicados
- Actualizar archivo Excel con mensajes nuevos
- Eliminar duplicado de Ernst Starhemberg
- Total: 64 mensajes únicos
- Mantener mensaje más completo por persona

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Mensajes_Antonio_limpio.xlsx
+++ b/Mensajes_Antonio_limpio.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="180">
   <si>
     <t>Nombre</t>
   </si>
@@ -40,12 +40,12 @@
     <t xml:space="preserve">Miguel </t>
   </si>
   <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
     <t>Carlos</t>
   </si>
   <si>
-    <t>SALVADOR</t>
-  </si>
-  <si>
     <t>Alberto</t>
   </si>
   <si>
@@ -76,6 +76,9 @@
     <t xml:space="preserve">Victoria </t>
   </si>
   <si>
+    <t>María</t>
+  </si>
+  <si>
     <t>Pablo</t>
   </si>
   <si>
@@ -94,9 +97,6 @@
     <t>Sergio</t>
   </si>
   <si>
-    <t>Alejandro</t>
-  </si>
-  <si>
     <t>Emilio</t>
   </si>
   <si>
@@ -136,36 +136,36 @@
     <t>Felipe</t>
   </si>
   <si>
+    <t xml:space="preserve">Luis </t>
+  </si>
+  <si>
+    <t>Veronica Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verónica </t>
+  </si>
+  <si>
+    <t>Ainara</t>
+  </si>
+  <si>
+    <t>Carmen</t>
+  </si>
+  <si>
+    <t>Jaime</t>
+  </si>
+  <si>
+    <t>Paulo</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Stella</t>
+  </si>
+  <si>
     <t>Luis</t>
   </si>
   <si>
-    <t xml:space="preserve">Luis </t>
-  </si>
-  <si>
-    <t>Veronica Maria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verónica </t>
-  </si>
-  <si>
-    <t>Ainara</t>
-  </si>
-  <si>
-    <t>Carmen</t>
-  </si>
-  <si>
-    <t>Jaime</t>
-  </si>
-  <si>
-    <t>Paulo</t>
-  </si>
-  <si>
-    <t>Ivan</t>
-  </si>
-  <si>
-    <t>Stella</t>
-  </si>
-  <si>
     <t>Antonio</t>
   </si>
   <si>
@@ -184,9 +184,6 @@
     <t>Gioia</t>
   </si>
   <si>
-    <t>maria</t>
-  </si>
-  <si>
     <t>ARIAS BERMUDEZ</t>
   </si>
   <si>
@@ -196,15 +193,15 @@
     <t>Arias</t>
   </si>
   <si>
+    <t>Artacho</t>
+  </si>
+  <si>
     <t>Aso</t>
   </si>
   <si>
     <t>Aso Miranda</t>
   </si>
   <si>
-    <t>BARDO</t>
-  </si>
-  <si>
     <t>Benbunan</t>
   </si>
   <si>
@@ -238,6 +235,9 @@
     <t xml:space="preserve">Entrecanales </t>
   </si>
   <si>
+    <t>Fanjul</t>
+  </si>
+  <si>
     <t>Fernandez Alvarez</t>
   </si>
   <si>
@@ -277,9 +277,6 @@
     <t>Hojman</t>
   </si>
   <si>
-    <t>Iborra  Broseta</t>
-  </si>
-  <si>
     <t>Iborra Broseta</t>
   </si>
   <si>
@@ -313,9 +310,6 @@
     <t>Nebrera</t>
   </si>
   <si>
-    <t>Paris</t>
-  </si>
-  <si>
     <t>París</t>
   </si>
   <si>
@@ -374,9 +368,6 @@
   </si>
   <si>
     <t>de la Torre</t>
-  </si>
-  <si>
-    <t>fanjul</t>
   </si>
   <si>
     <t>Querido Antonio,
@@ -400,6 +391,9 @@
 Miguel Arias</t>
   </si>
   <si>
+    <t>Antonio, desde que te conocí en Tokyo en 2019 ya vi que eras un líder nato y una gran persona. Muchas gracias por habernos dado tanto. Gracias a tu liderazgo has conseguido impactar positivamente muchas vidas. Has servido a la comunidad como nadie. Aquí nos tienes siempre. Te vamos a echar mucho de menos, crack! Te queremos! Abrazo fuerte</t>
+  </si>
+  <si>
     <t>Has conseguido llevar Endeavor España a otra dimensión! Gracias por todo lo que has aportado al emprendimiento  y gracias por haber contado con Andbank. Muchos éxitos en tu nueva etapa!</t>
   </si>
   <si>
@@ -442,6 +436,11 @@
     <t>Querido Antonio, 
 Te vamos a echar muchísimo de menos, espero que nos vistes con mucha pero que mucha frecuencia en la ofi. Te deseo lo mejor en esta nueva aventura, que es un claro ejemplo del que sigue lo consigue. Un abrazo enorme! 
 Vic</t>
+  </si>
+  <si>
+    <t>Te seguiremos acompañando allá donde vayas. 
+Un beso enorme y mucha suerte!! 
+María Fanjul</t>
   </si>
   <si>
     <t>Antonio! Justo tenía que estar en YPO y no pude venir, pero quería escribirte unas palabras. Recuerdo la primera vez que te vi hace ya casi 20 años en las oficinas de BCG cuando me dijiste como si nadad "me voy al MIT" y pensé "menudo crack" jaja... Quería darte las GRACIAS por lo que has hecho por el ecosistema emprendedor en España. Has llevado Endeavor al siguiente nivel de crecimiento y reputación y dejado una huella en muchísima gente! En lo personal ha sido un auténtico placer trabajar contigo. Pocas personas conozco con tanta distancia entre su brillantez y su ego. Tu generosidad con los demás es un ejemplo. Mucha suerte en esta nueva fase y espero poder conservar la amistad mucho tiempo! Aquí me tienes para lo que necesites! (compartimos consejos de emprender y de familia jajaja)</t>
@@ -497,10 +496,6 @@
     <t>Antonio querido, qué decirte... cuántas cosas vivimos juntos y cuánto aprendí de vos. Siempre te lo dije y te lo volveré a repetir, fuiste y serás un gran mentor para mi y estoy eternamente agradecida en cómo me abriste las puertas y me ayudaste a "volar". Es increíble todo lo que lograste estos años y el crecimiento exponencial que tuvo la organización gracias a vos y el gran equipo que armaste y lideraste. Se te va a extrañar mucho pero pero pero: once Endeavor, always Endeavor</t>
   </si>
   <si>
-    <t>Gracias por tu ayuda y dedicacion a este gran grupo de locos emprendedores.
-Un abrazo.</t>
-  </si>
-  <si>
     <t>Antonio eres un crack, te ira super bien en tu nuevo proyecto. 
 Gracias por compartir y ayudar tanto estos años. Un abrazo. Lucia.</t>
   </si>
@@ -537,11 +532,6 @@
   </si>
   <si>
     <t>Mucha suerte Antonio, te deseo todo lo mejor en tu nuevo camino. Dejas una comunidad Endeavor fuerte en España, construida en gran medida gracias a tu liderazgo y determinación, y siempre desde la humildad y generosidad. Enhorabuena y un fuerte abrazo!! Pablo Nebrera</t>
-  </si>
-  <si>
-    <t>¡Muchísimas gracias por todos estos años! 
-un fuerte abrazo
-Luis</t>
   </si>
   <si>
     <t>¡Muchísimas gracias por todos estos años!
@@ -599,8 +589,10 @@
 Antonio Serrano</t>
   </si>
   <si>
-    <t xml:space="preserve">Gracias por todo Antonio!
-</t>
+    <t>Querido Antonio,
+Gracias por estos tres años juntos en Endeavor — por tu liderazgo, pero sobre todo por tu cercanía, humanidad y empatía. He y hemos aprendido mucho de ti. Te vamos a echar muchísimo de menos, aunque estoy seguro de que nos veremos pronto (y más de una vez). Eres una grandisima persona.
+Un abrazo enorme y muchísima suerte en todo lo que te espera,
+Ernst</t>
   </si>
   <si>
     <t>Antonio, enhorabuena por el impresionante legado que dejas, y gracias por hacer hueco para que otro pueda disfrutar de este trabajazo :)
@@ -623,21 +615,13 @@
     <t>Gracias por todo lo que has hecho por Endeavor España y por nosotros en CARTO.
 Tu apoyo, visión y generosidad han dejado huella.
 Más allá del trabajo, es un auténtico gusto tenerte cerca. Jatorre!</t>
-  </si>
-  <si>
-    <t>Te seguiremos acompañando allá donde vayas. 
-Un beso enorme y mucha suerte!! 
-María Fanjul</t>
-  </si>
-  <si>
-    <t>https://kvhpaojlvwwetdzqhbqf.supabase.co/storage/v1/object/public/farewell-videos/1754218034795-IMG_5284.MOV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -652,13 +636,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -693,22 +670,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1001,7 +972,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1026,10 +997,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1037,10 +1008,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1051,7 +1022,7 @@
         <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1059,10 +1030,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1070,21 +1041,21 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1092,10 +1063,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>184</v>
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1103,10 +1074,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1114,10 +1085,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1125,10 +1096,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1136,10 +1107,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1147,10 +1118,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1158,10 +1129,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1169,10 +1140,10 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1180,10 +1151,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1191,10 +1162,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1202,10 +1173,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1213,10 +1184,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1224,10 +1195,10 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1235,10 +1206,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1246,32 +1217,32 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1279,10 +1250,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1290,10 +1261,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1301,65 +1272,65 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1367,10 +1338,10 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1378,10 +1349,10 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1389,10 +1360,10 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1400,10 +1371,10 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1411,10 +1382,10 @@
         <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C37" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1422,10 +1393,10 @@
         <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1433,10 +1404,10 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1444,10 +1415,10 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1455,10 +1426,10 @@
         <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1466,10 +1437,10 @@
         <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1477,10 +1448,10 @@
         <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1488,21 +1459,21 @@
         <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C45" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1510,10 +1481,10 @@
         <v>40</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C46" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1521,10 +1492,10 @@
         <v>41</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C47" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1532,10 +1503,10 @@
         <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C48" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1543,10 +1514,10 @@
         <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1554,10 +1525,10 @@
         <v>44</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C50" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1565,54 +1536,54 @@
         <v>45</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C52" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C53" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C55" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1620,10 +1591,10 @@
         <v>48</v>
       </c>
       <c r="B56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C56" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1631,126 +1602,101 @@
         <v>49</v>
       </c>
       <c r="B57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C57" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C58" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C59" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C60" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B61" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C61" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C62" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="B63" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C63" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C64" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C65" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>6</v>
-      </c>
-      <c r="B66" t="s">
-        <v>119</v>
-      </c>
-      <c r="C66" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
-        <v>56</v>
-      </c>
-      <c r="B67" t="s">
-        <v>120</v>
-      </c>
-      <c r="C67" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Eliminar duplicado de Carlos Aso
- Había dos registros: 'Carlos Aso' y 'Carlos Aso Miranda'
- Ambos tenían el mismo mensaje idéntico
- Mantener 'Carlos Aso Miranda' (nombre completo)
- Total: 63 mensajes únicos

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Mensajes_Antonio_limpio.xlsx
+++ b/Mensajes_Antonio_limpio.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="179">
   <si>
     <t>Nombre</t>
   </si>
@@ -194,9 +194,6 @@
   </si>
   <si>
     <t>Artacho</t>
-  </si>
-  <si>
-    <t>Aso</t>
   </si>
   <si>
     <t>Aso Miranda</t>
@@ -972,7 +969,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1000,7 +997,7 @@
         <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1011,7 +1008,7 @@
         <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1022,7 +1019,7 @@
         <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1033,7 +1030,7 @@
         <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1044,7 +1041,7 @@
         <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1055,12 +1052,12 @@
         <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>61</v>
@@ -1071,7 +1068,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>62</v>
@@ -1082,7 +1079,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>63</v>
@@ -1093,7 +1090,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
@@ -1104,7 +1101,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>65</v>
@@ -1115,7 +1112,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>66</v>
@@ -1126,7 +1123,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>67</v>
@@ -1137,7 +1134,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>68</v>
@@ -1148,7 +1145,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>69</v>
@@ -1159,7 +1156,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>70</v>
@@ -1170,7 +1167,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>71</v>
@@ -1181,7 +1178,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>72</v>
@@ -1192,7 +1189,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>73</v>
@@ -1203,7 +1200,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>74</v>
@@ -1214,7 +1211,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>75</v>
@@ -1225,7 +1222,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>76</v>
@@ -1236,7 +1233,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>77</v>
@@ -1247,7 +1244,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>78</v>
@@ -1258,7 +1255,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>79</v>
@@ -1269,7 +1266,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
         <v>80</v>
@@ -1280,7 +1277,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>81</v>
@@ -1291,7 +1288,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
         <v>82</v>
@@ -1302,7 +1299,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>83</v>
@@ -1313,7 +1310,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>84</v>
@@ -1324,7 +1321,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>85</v>
@@ -1346,10 +1343,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" t="s">
         <v>149</v>
@@ -1357,7 +1354,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
         <v>87</v>
@@ -1368,7 +1365,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
         <v>88</v>
@@ -1379,7 +1376,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
         <v>89</v>
@@ -1390,7 +1387,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
         <v>90</v>
@@ -1401,7 +1398,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
         <v>91</v>
@@ -1412,7 +1409,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>92</v>
@@ -1423,7 +1420,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
         <v>93</v>
@@ -1434,7 +1431,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
         <v>94</v>
@@ -1445,7 +1442,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B43" t="s">
         <v>95</v>
@@ -1456,7 +1453,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
         <v>96</v>
@@ -1467,7 +1464,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
         <v>97</v>
@@ -1478,7 +1475,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B46" t="s">
         <v>98</v>
@@ -1489,18 +1486,18 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
         <v>99</v>
       </c>
       <c r="C47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B48" t="s">
         <v>100</v>
@@ -1511,7 +1508,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
         <v>101</v>
@@ -1522,7 +1519,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B50" t="s">
         <v>102</v>
@@ -1533,7 +1530,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B51" t="s">
         <v>103</v>
@@ -1544,7 +1541,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B52" t="s">
         <v>104</v>
@@ -1555,7 +1552,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B53" t="s">
         <v>105</v>
@@ -1566,7 +1563,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B54" t="s">
         <v>106</v>
@@ -1577,7 +1574,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B55" t="s">
         <v>107</v>
@@ -1588,7 +1585,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B56" t="s">
         <v>108</v>
@@ -1599,7 +1596,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B57" t="s">
         <v>109</v>
@@ -1610,7 +1607,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B58" t="s">
         <v>110</v>
@@ -1621,7 +1618,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B59" t="s">
         <v>111</v>
@@ -1632,7 +1629,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B60" t="s">
         <v>112</v>
@@ -1643,7 +1640,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="B61" t="s">
         <v>113</v>
@@ -1654,7 +1651,7 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="B62" t="s">
         <v>114</v>
@@ -1665,7 +1662,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B63" t="s">
         <v>115</v>
@@ -1676,24 +1673,13 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="B64" t="s">
         <v>116</v>
       </c>
       <c r="C64" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
-        <v>6</v>
-      </c>
-      <c r="B65" t="s">
-        <v>117</v>
-      </c>
-      <c r="C65" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>